<commit_message>
update baseline for revised destination types
</commit_message>
<xml_diff>
--- a/output/20mn baseline area coverage.xlsx
+++ b/output/20mn baseline area coverage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\MEGAsync\Steve\RMIT JIBE\20mnMelbourne\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518C8D30-CA2C-425F-8AF3-493FDC812BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08418ACA-F542-48DE-8F36-35FC378414D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17370" yWindow="-14955" windowWidth="19635" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="-13020" windowWidth="13635" windowHeight="10725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20mn baseline area coverage" sheetId="1" r:id="rId1"/>
@@ -20,81 +20,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Restaurant or cafe within 400m</t>
-  </si>
-  <si>
-    <t>Supermarket within 800m</t>
-  </si>
-  <si>
-    <t>Bakery within 800m</t>
-  </si>
-  <si>
-    <t>Pharmacy within 800m</t>
-  </si>
-  <si>
-    <t>Post office within 800m</t>
-  </si>
-  <si>
-    <t>Local park within 400m</t>
-  </si>
-  <si>
-    <t>Community centre within 800m</t>
-  </si>
-  <si>
-    <t>Childcare centre within 800m</t>
-  </si>
-  <si>
-    <t>Primary school within 800m</t>
-  </si>
-  <si>
-    <t>Community health centre within 800m</t>
-  </si>
-  <si>
-    <t>Maternal &amp; child health centre within 800m</t>
-  </si>
-  <si>
-    <t>Large NACs</t>
-  </si>
-  <si>
-    <t>Medium NACs</t>
-  </si>
-  <si>
-    <t>Small NACs</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Melbourne</t>
   </si>
   <si>
-    <t>All NACs</t>
-  </si>
-  <si>
-    <t>Bus within 400m, tram with 600m or train within 800m</t>
-  </si>
-  <si>
-    <t>Kindergarten within 800m</t>
-  </si>
-  <si>
-    <t>District sports facility within 800m</t>
-  </si>
-  <si>
-    <t>GP within 400m</t>
-  </si>
-  <si>
-    <t>Dentist within 800m</t>
-  </si>
-  <si>
     <t>Number of residences</t>
   </si>
   <si>
-    <t>Butcher within 800m</t>
-  </si>
-  <si>
-    <t>Convenience store or supermarket within 400m</t>
-  </si>
-  <si>
     <t>Percentage of dwellings within specified walking distance of destination type</t>
+  </si>
+  <si>
+    <t>Reachable within 800m walking distance</t>
+  </si>
+  <si>
+    <t>Reachable within 400m walking distance</t>
+  </si>
+  <si>
+    <t>Reachable within 400m (bus), 600m (tram) or 800m (train) walking distance</t>
+  </si>
+  <si>
+    <t>Supermarket</t>
+  </si>
+  <si>
+    <t>Pharmacy</t>
+  </si>
+  <si>
+    <t>Post office</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>Maternal &amp; child health centre</t>
+  </si>
+  <si>
+    <t>Dentist</t>
+  </si>
+  <si>
+    <t>Childcare centre</t>
+  </si>
+  <si>
+    <t>Kindergarten</t>
+  </si>
+  <si>
+    <t>Primary school</t>
+  </si>
+  <si>
+    <t>Community centre or library</t>
+  </si>
+  <si>
+    <t>Convenience store or supermarket</t>
+  </si>
+  <si>
+    <t>Restaurant or cafe</t>
+  </si>
+  <si>
+    <t>Local park</t>
+  </si>
+  <si>
+    <t>Bus stop, tram stop or train station</t>
+  </si>
+  <si>
+    <t>All ACs</t>
+  </si>
+  <si>
+    <t>Large ACs</t>
+  </si>
+  <si>
+    <t>Medium ACs</t>
+  </si>
+  <si>
+    <t>Small ACs</t>
   </si>
 </sst>
 </file>
@@ -722,7 +719,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -732,9 +729,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -764,6 +758,15 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1148,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F21"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -1163,420 +1166,373 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>40.591830000000002</v>
+      </c>
+      <c r="C4" s="5">
+        <v>72.436520000000002</v>
+      </c>
+      <c r="D4" s="5">
+        <v>89.401340000000005</v>
+      </c>
+      <c r="E4" s="5">
+        <v>71.433019999999999</v>
+      </c>
+      <c r="F4" s="6">
+        <v>39.645650000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5">
+        <v>31.790959999999998</v>
+      </c>
+      <c r="C5" s="5">
+        <v>51.777709999999999</v>
+      </c>
+      <c r="D5" s="5">
+        <v>60.337679999999999</v>
+      </c>
+      <c r="E5" s="5">
+        <v>52.834000000000003</v>
+      </c>
+      <c r="F5" s="6">
+        <v>32.085650000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
+        <v>17.62313</v>
+      </c>
+      <c r="C6" s="5">
+        <v>30.95505</v>
+      </c>
+      <c r="D6" s="5">
+        <v>37.835650000000001</v>
+      </c>
+      <c r="E6" s="5">
+        <v>29.764669999999999</v>
+      </c>
+      <c r="F6" s="6">
+        <v>18.681999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
+        <v>51.336469999999998</v>
+      </c>
+      <c r="C7" s="5">
+        <v>78.534000000000006</v>
+      </c>
+      <c r="D7" s="5">
+        <v>89.469390000000004</v>
+      </c>
+      <c r="E7" s="5">
+        <v>79.19041</v>
+      </c>
+      <c r="F7" s="6">
+        <v>57.89922</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5">
+        <v>24.748750000000001</v>
+      </c>
+      <c r="C8" s="5">
+        <v>36.413800000000002</v>
+      </c>
+      <c r="D8" s="5">
+        <v>40.906559999999999</v>
+      </c>
+      <c r="E8" s="5">
+        <v>37.171709999999997</v>
+      </c>
+      <c r="F8" s="6">
+        <v>30.53585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5">
+        <v>42.428249999999998</v>
+      </c>
+      <c r="C9" s="5">
+        <v>67.421700000000001</v>
+      </c>
+      <c r="D9" s="5">
+        <v>81.441590000000005</v>
+      </c>
+      <c r="E9" s="5">
+        <v>62.265439999999998</v>
+      </c>
+      <c r="F9" s="6">
+        <v>44.544379999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5">
+        <v>78.132720000000006</v>
+      </c>
+      <c r="C10" s="5">
+        <v>92.006309999999999</v>
+      </c>
+      <c r="D10" s="5">
+        <v>94.147040000000004</v>
+      </c>
+      <c r="E10" s="5">
+        <v>92.758049999999997</v>
+      </c>
+      <c r="F10" s="6">
+        <v>88.659009999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5">
+        <v>39.379190000000001</v>
+      </c>
+      <c r="C11" s="5">
+        <v>48.26961</v>
+      </c>
+      <c r="D11" s="5">
+        <v>47.456859999999999</v>
+      </c>
+      <c r="E11" s="5">
+        <v>52.200899999999997</v>
+      </c>
+      <c r="F11" s="6">
+        <v>50.114609999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="B12" s="5">
+        <v>46.709609999999998</v>
+      </c>
+      <c r="C12" s="5">
+        <v>58.616199999999999</v>
+      </c>
+      <c r="D12" s="5">
+        <v>59.441749999999999</v>
+      </c>
+      <c r="E12" s="5">
+        <v>67.425030000000007</v>
+      </c>
+      <c r="F12" s="6">
+        <v>58.088529999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="B13" s="5">
+        <v>21.777000000000001</v>
+      </c>
+      <c r="C13" s="5">
+        <v>35.651519999999998</v>
+      </c>
+      <c r="D13" s="5">
+        <v>46.221220000000002</v>
+      </c>
+      <c r="E13" s="5">
+        <v>29.864339999999999</v>
+      </c>
+      <c r="F13" s="6">
+        <v>21.269390000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5">
+        <v>24.965409999999999</v>
+      </c>
+      <c r="C15" s="5">
+        <v>45.275210000000001</v>
+      </c>
+      <c r="D15" s="5">
+        <v>52.511899999999997</v>
+      </c>
+      <c r="E15" s="5">
+        <v>35.923079999999999</v>
+      </c>
+      <c r="F15" s="6">
+        <v>37.333979999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="5">
         <v>31.56897</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C16" s="5">
         <v>54.930219999999998</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D16" s="5">
         <v>62.064909999999998</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E16" s="5">
         <v>45.742199999999997</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F16" s="6">
         <v>49.572400000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="23" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="6">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="5">
+        <v>74.77646</v>
+      </c>
+      <c r="C17" s="5">
+        <v>78.289019999999994</v>
+      </c>
+      <c r="D17" s="5">
+        <v>80.627189999999999</v>
+      </c>
+      <c r="E17" s="5">
+        <v>78.977919999999997</v>
+      </c>
+      <c r="F17" s="6">
+        <v>74.796589999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5">
         <v>75.760379999999998</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C19" s="5">
         <v>92.169129999999996</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D19" s="5">
         <v>94.012500000000003</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E19" s="5">
         <v>91.762299999999996</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F19" s="6">
         <v>91.08314</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="20" spans="1:10" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6">
-        <v>40.591830000000002</v>
-      </c>
-      <c r="C5" s="6">
-        <v>72.436520000000002</v>
-      </c>
-      <c r="D5" s="6">
-        <v>89.401340000000005</v>
-      </c>
-      <c r="E5" s="6">
-        <v>71.433019999999999</v>
-      </c>
-      <c r="F5" s="7">
-        <v>39.645650000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="23" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="6">
-        <v>24.965409999999999</v>
-      </c>
-      <c r="C6" s="6">
-        <v>45.275210000000001</v>
-      </c>
-      <c r="D6" s="6">
-        <v>52.511899999999997</v>
-      </c>
-      <c r="E6" s="6">
-        <v>35.923079999999999</v>
-      </c>
-      <c r="F6" s="7">
-        <v>37.333979999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="6">
-        <v>8.7349599999999992</v>
-      </c>
-      <c r="C7" s="6">
-        <v>15.72162</v>
-      </c>
-      <c r="D7" s="6">
-        <v>20.820650000000001</v>
-      </c>
-      <c r="E7" s="6">
-        <v>10.306889999999999</v>
-      </c>
-      <c r="F7" s="7">
-        <v>10.20181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6">
-        <v>18.96294</v>
-      </c>
-      <c r="C8" s="6">
-        <v>34.683079999999997</v>
-      </c>
-      <c r="D8" s="6">
-        <v>43.196449999999999</v>
-      </c>
-      <c r="E8" s="6">
-        <v>31.84836</v>
-      </c>
-      <c r="F8" s="7">
-        <v>20.998940000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6">
-        <v>31.790959999999998</v>
-      </c>
-      <c r="C9" s="6">
-        <v>51.777709999999999</v>
-      </c>
-      <c r="D9" s="6">
-        <v>60.337679999999999</v>
-      </c>
-      <c r="E9" s="6">
-        <v>52.834000000000003</v>
-      </c>
-      <c r="F9" s="7">
-        <v>32.085650000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="6">
-        <v>17.62313</v>
-      </c>
-      <c r="C10" s="6">
-        <v>30.95505</v>
-      </c>
-      <c r="D10" s="6">
-        <v>37.835650000000001</v>
-      </c>
-      <c r="E10" s="6">
-        <v>29.764669999999999</v>
-      </c>
-      <c r="F10" s="7">
-        <v>18.681999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="6">
-        <v>74.77646</v>
-      </c>
-      <c r="C11" s="6">
-        <v>78.289019999999994</v>
-      </c>
-      <c r="D11" s="6">
-        <v>80.627189999999999</v>
-      </c>
-      <c r="E11" s="6">
-        <v>78.977919999999997</v>
-      </c>
-      <c r="F11" s="7">
-        <v>74.796589999999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="6">
-        <v>14.48845</v>
-      </c>
-      <c r="C12" s="6">
-        <v>21.213170000000002</v>
-      </c>
-      <c r="D12" s="6">
-        <v>23.400680000000001</v>
-      </c>
-      <c r="E12" s="6">
-        <v>21.89489</v>
-      </c>
-      <c r="F12" s="7">
-        <v>17.192889999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="6">
-        <v>78.132720000000006</v>
-      </c>
-      <c r="C13" s="6">
-        <v>92.006309999999999</v>
-      </c>
-      <c r="D13" s="6">
-        <v>94.147040000000004</v>
-      </c>
-      <c r="E13" s="6">
-        <v>92.758049999999997</v>
-      </c>
-      <c r="F13" s="7">
-        <v>88.659009999999995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6">
-        <v>39.379190000000001</v>
-      </c>
-      <c r="C14" s="6">
-        <v>48.26961</v>
-      </c>
-      <c r="D14" s="6">
-        <v>47.456859999999999</v>
-      </c>
-      <c r="E14" s="6">
-        <v>52.200899999999997</v>
-      </c>
-      <c r="F14" s="7">
-        <v>50.114609999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="6">
-        <v>46.709609999999998</v>
-      </c>
-      <c r="C15" s="6">
-        <v>58.616199999999999</v>
-      </c>
-      <c r="D15" s="6">
-        <v>59.441749999999999</v>
-      </c>
-      <c r="E15" s="6">
-        <v>67.425030000000007</v>
-      </c>
-      <c r="F15" s="7">
-        <v>58.088529999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="6">
-        <v>43.659190000000002</v>
-      </c>
-      <c r="C16" s="6">
-        <v>49.535420000000002</v>
-      </c>
-      <c r="D16" s="6">
-        <v>50.327469999999998</v>
-      </c>
-      <c r="E16" s="6">
-        <v>49.615400000000001</v>
-      </c>
-      <c r="F16" s="7">
-        <v>49.999839999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6">
-        <v>2.153826</v>
-      </c>
-      <c r="C17" s="6">
-        <v>3.8170199999999999</v>
-      </c>
-      <c r="D17" s="6">
-        <v>5.1632170000000004</v>
-      </c>
-      <c r="E17" s="6">
-        <v>2.5833080000000002</v>
-      </c>
-      <c r="F17" s="7">
-        <v>3.067272</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="23" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6">
-        <v>24.748750000000001</v>
-      </c>
-      <c r="C18" s="6">
-        <v>36.413800000000002</v>
-      </c>
-      <c r="D18" s="6">
-        <v>40.906559999999999</v>
-      </c>
-      <c r="E18" s="6">
-        <v>37.171709999999997</v>
-      </c>
-      <c r="F18" s="7">
-        <v>30.53585</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="6">
-        <v>21.36065</v>
-      </c>
-      <c r="C19" s="6">
-        <v>38.034179999999999</v>
-      </c>
-      <c r="D19" s="6">
-        <v>45.48433</v>
-      </c>
-      <c r="E19" s="6">
-        <v>34.047939999999997</v>
-      </c>
-      <c r="F19" s="7">
-        <v>26.91911</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="6">
-        <v>42.428249999999998</v>
-      </c>
-      <c r="C20" s="6">
-        <v>67.421700000000001</v>
-      </c>
-      <c r="D20" s="6">
-        <v>81.441590000000005</v>
-      </c>
-      <c r="E20" s="6">
-        <v>62.265439999999998</v>
-      </c>
-      <c r="F20" s="7">
-        <v>44.544379999999997</v>
+      <c r="B20" s="8">
+        <v>2274046</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1082153</v>
+      </c>
+      <c r="D20" s="8">
+        <v>697937</v>
+      </c>
+      <c r="E20" s="8">
+        <v>227770</v>
+      </c>
+      <c r="F20" s="9">
+        <v>303201</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="9">
-        <v>2274046</v>
-      </c>
-      <c r="C21" s="9">
-        <v>1082153</v>
-      </c>
-      <c r="D21" s="9">
-        <v>697937</v>
-      </c>
-      <c r="E21" s="9">
-        <v>227770</v>
-      </c>
-      <c r="F21" s="10">
-        <v>303201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J22" s="11"/>
+      <c r="J21" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A18:F18"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:F20">
+  <conditionalFormatting sqref="B4:F13 B15:F17 B19:F19">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>80</formula>
     </cfRule>

</xml_diff>